<commit_message>
Updates to cardiovascular and endocrine matrices. Updates to cardiovascular and endocrine methodology reports.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/EndocrineValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/EndocrineValidation.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngine\data\human\adult\validation\Scenarios\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9327BD-A6B5-480B-89EE-6064652B1D3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="-210" windowWidth="20010" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,17 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$B$1:$K$4</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -168,7 +184,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -711,7 +727,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -832,6 +848,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -861,16 +880,16 @@
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Bad 2" xfId="45"/>
-    <cellStyle name="Bad 3" xfId="47"/>
-    <cellStyle name="Bad 4" xfId="43"/>
+    <cellStyle name="Bad 2" xfId="45" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Bad 3" xfId="47" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Bad 4" xfId="43" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Good 2" xfId="44"/>
-    <cellStyle name="Good 3" xfId="46"/>
-    <cellStyle name="Good 4" xfId="42"/>
+    <cellStyle name="Good 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Good 3" xfId="46" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Good 4" xfId="42" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
     <cellStyle name="Heading 1" xfId="5" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="6" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="7" builtinId="18" customBuiltin="1"/>
@@ -890,6 +909,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -938,7 +960,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -971,9 +993,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1006,6 +1045,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1181,7 +1237,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1393,7 +1449,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1468,11 +1524,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection sqref="A1:Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,13 +1543,13 @@
     <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.140625" customWidth="1"/>
     <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
     <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="26" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" style="26" customWidth="1"/>
     <col min="14" max="14" width="23" style="26" customWidth="1"/>
-    <col min="15" max="15" width="19.85546875" style="26" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" style="26" customWidth="1"/>
     <col min="16" max="16" width="23" style="26" customWidth="1"/>
-    <col min="17" max="17" width="3" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" customWidth="1"/>
     <col min="18" max="18" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
   </cols>
@@ -1673,7 +1729,7 @@
       <c r="O4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="P4" s="40" t="s">
+      <c r="P4" s="6" t="s">
         <v>31</v>
       </c>
       <c r="Q4" s="3" t="s">
@@ -1779,7 +1835,7 @@
       <c r="O6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="P6" s="6" t="s">
+      <c r="P6" s="42" t="s">
         <v>41</v>
       </c>
       <c r="Q6" s="3" t="s">
@@ -1898,21 +1954,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D00DDCF912707249810263345C6FBCAE" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="05fc12c866532ec63d2052ef81b63530">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="711b5f35d88f7f6ebfe284b0f73f4393">
     <xsd:element name="properties">
@@ -2026,17 +2067,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6320210A-C44C-4B82-8349-5A58CB3B5A77}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{000C402D-5B8F-44E9-B6EC-AD906C5241AB}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2050,17 +2107,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{000C402D-5B8F-44E9-B6EC-AD906C5241AB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6320210A-C44C-4B82-8349-5A58CB3B5A77}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Documentation updates. Mainly validation results.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/EndocrineValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/EndocrineValidation.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngine\data\human\adult\validation\Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\documentation\source\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9327BD-A6B5-480B-89EE-6064652B1D3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD503662-5E32-4ADB-8954-ED4F7B6984E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26370" yWindow="3495" windowWidth="26970" windowHeight="24390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Key" sheetId="3" r:id="rId2"/>
-    <sheet name="Acute Stress" sheetId="4" r:id="rId3"/>
+    <sheet name="Acute Stress" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$B$1:$K$4</definedName>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="43">
   <si>
     <t xml:space="preserve">Scenario </t>
   </si>
@@ -43,9 +42,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Key</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -70,21 +66,6 @@
     <t>|&lt;span class="success"&gt;</t>
   </si>
   <si>
-    <t>Good agreement: correct trends or &lt;10% deviation from expected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|&lt;span class="warning"&gt; </t>
-  </si>
-  <si>
-    <t>Some deviation: correct trend and/or &lt;30% deviation from expected</t>
-  </si>
-  <si>
-    <t>|&lt;span class="danger"&gt;</t>
-  </si>
-  <si>
-    <t>Poor agreement: incorrect trends or &gt;30% deviation from expected</t>
-  </si>
-  <si>
     <t>Good</t>
   </si>
   <si>
@@ -179,6 +160,9 @@
   </si>
   <si>
     <t>.034 ug/L @cite wortsman1984adrenomedullary</t>
+  </si>
+  <si>
+    <t>|&lt;span class="warning"&gt;</t>
   </si>
 </sst>
 </file>
@@ -727,7 +711,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -760,33 +744,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -798,26 +755,22 @@
     <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -835,13 +788,10 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="44" applyBorder="1" applyAlignment="1">
@@ -851,6 +801,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -918,9 +874,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -958,9 +914,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -993,26 +949,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1045,26 +984,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1244,7 +1166,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,152 +1176,152 @@
     <col min="3" max="3" width="1.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="56.42578125" style="4" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="29" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="29" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="29"/>
+    <col min="6" max="6" width="9.140625" style="18" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="18" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="18"/>
     <col min="12" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>5</v>
+      <c r="A1" s="25" t="s">
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="36" t="s">
-        <v>5</v>
+      <c r="C1" s="25" t="s">
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="24" t="s">
-        <v>5</v>
+      <c r="E1" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
-        <v>5</v>
+      <c r="A3" s="24" t="s">
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="21">
+        <v>21</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="12">
+        <v>15</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="13">
+        <v>2</v>
+      </c>
+      <c r="I3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="22">
-        <v>1</v>
-      </c>
-      <c r="I3" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="30">
+      <c r="J3" s="19">
+        <v>4</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="14">
+        <f>F3</f>
+        <v>15</v>
+      </c>
+      <c r="G4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="H4" s="13">
+        <f>H3</f>
+        <v>2</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="19">
+        <f>J3</f>
+        <v>4</v>
+      </c>
+      <c r="K4" s="16" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="23">
-        <f>F3</f>
-        <v>13</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="22">
-        <f>H3</f>
-        <v>1</v>
-      </c>
-      <c r="I4" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="30">
-        <f>J3</f>
-        <v>6</v>
-      </c>
-      <c r="K4" s="25" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1449,503 +1371,429 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:S8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Q8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2" style="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1"/>
-    <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" style="26" customWidth="1"/>
-    <col min="14" max="14" width="23" style="26" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" style="26" customWidth="1"/>
-    <col min="16" max="16" width="23" style="26" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" customWidth="1"/>
-    <col min="18" max="18" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" style="31" customWidth="1"/>
+    <col min="10" max="10" width="23" style="31" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" style="31" customWidth="1"/>
+    <col min="12" max="12" width="23" style="31" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" style="31" customWidth="1"/>
+    <col min="14" max="14" width="23" style="31" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" style="31" customWidth="1"/>
+    <col min="16" max="16" width="25.42578125" style="31" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" style="31" customWidth="1"/>
+    <col min="18" max="18" width="23.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" style="31" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
+      <c r="A1" s="18"/>
+      <c r="B1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
     </row>
     <row r="2" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
+      <c r="A2" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
+      <c r="C2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>5</v>
+        <v>22</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>5</v>
+        <v>23</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>5</v>
+        <v>24</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>5</v>
+      <c r="A3" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
+      <c r="A4" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="F4" s="9">
         <v>20</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>5</v>
+      <c r="G4" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="H4" s="9">
         <v>210</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="O4" s="3" t="s">
+      <c r="I4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="P4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="Q4" s="8" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="5" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="B5" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="F5" s="9">
         <v>220</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>5</v>
+      <c r="G5" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="H5" s="9">
         <v>610</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N5" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P5" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>6</v>
+      <c r="I5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
+      <c r="A6" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="F6" s="9">
         <v>620</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>5</v>
+      <c r="G6" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="H6" s="9">
         <v>810</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="41" t="s">
+      <c r="I6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="P6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N6" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="P6" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="Q6" s="8" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="7" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="B7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="F7" s="9">
         <v>820</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>5</v>
+      <c r="G7" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="H7" s="9">
         <v>1210</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N7" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P7" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="I7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="P7" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q7" s="8" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="8" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="B8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="F8" s="9">
         <v>1220</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>5</v>
+      <c r="G8" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="H8" s="9">
         <v>1410</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L8" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N8" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P8" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q8" s="3" t="s">
+      <c r="I8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="8" t="s">
         <v>6</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="P8" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1954,6 +1802,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D00DDCF912707249810263345C6FBCAE" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="05fc12c866532ec63d2052ef81b63530">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="711b5f35d88f7f6ebfe284b0f73f4393">
     <xsd:element name="properties">
@@ -2067,22 +1930,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6320210A-C44C-4B82-8349-5A58CB3B5A77}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1B20E2-65A5-4DC5-B5E1-EAEF16402220}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{000C402D-5B8F-44E9-B6EC-AD906C5241AB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2096,27 +1967,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1B20E2-65A5-4DC5-B5E1-EAEF16402220}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6320210A-C44C-4B82-8349-5A58CB3B5A77}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>